<commit_message>
changes weeks ago TT
</commit_message>
<xml_diff>
--- a/backend/scraping_result.xlsx
+++ b/backend/scraping_result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B21"/>
+  <dimension ref="A2:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,29 +443,211 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fresh Salad Greens
+          <t xml:space="preserve">THREE-SIXTY Protein
 </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
           <t xml:space="preserve">
-BYO Poke Bowl CV
-$11.50
-Romaine Lettuce
-Spring Mix
-Unseasoned Sticky Rice</t>
+Beef
+$4.50
+Lemongrass Shrimp
+$4.50
+Sliced Chicken
+$3.50
+Tofu w/ Plum Sauce
+$3.00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t xml:space="preserve">THREE-SIXTY Sauces
+</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Kung Pao Sauce
+Spicy Chili Dragon Sauce
+Sweet Chili Orange Sauce
+Szechuan Sauce</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">THREE-SIXTY Base
+</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Forbidden Rice
+Rice Noodles
+Yakisoba Noodle</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">360 Global Add ons
+</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Garlic Chili Oil
+Wonton Strips</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fusion Grill Styles
+</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Breakfast Smashburger
+$9.50
+California Burrito
+$10.00
+Triton Style
+$8.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fusion Grill Burger Patty
+</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Chicken Smash Patty
+$1.00
+Chipotle Black Bean
+Halal Beef Burger Patty
+Marinated Chicken Breast
+$1.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Soup
+</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Chicken &amp; Wild Rice Soup
+$4.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh Signature Salads
+</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Greek Salad
+$7.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fusion Grill Add ons
+</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Avocado
+$1.75
+Cheddar Cheese
+$1.00
+Provolone Cheese
+$1.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh Salad Dressings
+</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Spicy Mayo
+Balsamic Vinaigrette
+Buttermilk Ranch Dressing
+Caesar Dressing
+Italian Dressing
+Jalapeno Ranch
+Lava Sauce</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">THREE-SIXTY Vegetables
+</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Baby Corn
+Red Onions
+Shiitake Mushrooms
+Sliced Carrots
+Sliced Green Onion
+Sliced Red Bell Pepper
+Snap Peas
+Steamed Broccoli
+Water Chestnuts
+Bamboo Shoots
+Jalapenos</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t xml:space="preserve">Fresh Salad Proteins
 </t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Cage Free Hard Boiled Egg
@@ -481,14 +663,37 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">THREE-SIXTY Bowls
+</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Beef Bowl
+$10.00
+Chicken Bowl
+$9.00
+Shrimp Bowl
+$10.00
+Tofu Bowl
+$8.50
+Vegetable Bowl
+$6.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
         <is>
           <t xml:space="preserve">Fresh Salad Ingredients
 </t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t xml:space="preserve">
 1/4 Avocado
@@ -509,322 +714,21 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fresh Salad Dressings
-</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Balsamic Vinaigrette
-Buttermilk Ranch Dressing
-Caesar Dressing
-Italian Dressing
-Jalapeno Ranch
-Lava Sauce
-Spicy Mayo</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fusion Grill Styles
-</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Breakfast Smashburger
-$9.50
-California Burrito
-$10.00
-Triton Style
-$8.50</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fusion Grill Burger Patty
-</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Chicken Smash Patty
-$1.00
-Chipotle Black Bean
-Halal Beef Burger Patty
-Marinated Chicken Breast
-$1.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fusion Grill Add ons
-</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Avocado
-$1.75
-Cheddar Cheese
-$1.00
-Provolone Cheese
-$1.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fusion Sides
-</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Carne Asada Loaded Fries
-$9.00
-Chicken Tenders
-$6.25
-French Fries
-$3.00
-Grilled Salmon
-$6.00
-Marinated Chicken Breast
-$5.75</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">THREE-SIXTY Bowls
-</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-BBQ Lemongrass Tofu Bowl
-$8.50
-Beef Bowl
-$10.00
-Chicken Bowl
-$9.00
-Shrimp Bowl
-$10.00
-Vegetable Bowl
-$6.50</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">THREE-SIXTY Base
-</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Forbidden Rice
-Rice Noodles
-Yakisoba Noodle</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">THREE-SIXTY Protein
-</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Beef
-$4.50
-Lemongrass Shrimp
-$4.50
-Sliced Chicken
-$3.50
-Tofu w/ Plum Sauce
-$3.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">THREE-SIXTY Vegetables
-</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Baby Corn
-Bamboo Shoots
-Jalapenos
-Red Onions
-Shiitake Mushrooms
-Sliced Carrots
-Sliced Green Onion
-Sliced Red Bell Pepper
-Snap Peas
-Steamed Broccoli
-Water Chestnuts</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">THREE-SIXTY Sauces
-</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Kung Pao Sauce
-Spicy Chili Dragon Sauce
-Sweet Chili Orange Sauce
-Szechuan Sauce</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">360 Global Add ons
-</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Garlic Chili Oil
-Wonton Strips</t>
-        </is>
-      </c>
-    </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Soup
+          <t xml:space="preserve">Fresh Salad Greens
 </t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Chicken Pozole Verde
-$4.25</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fusion Specials
-</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Buffalo Wings and Fries
-$12.00
-CV Spicy Chicken Sandwich
-$9.50
-Carne Asada Loaded Fries
-$9.00
-Chicken Loaded French Fries
-$9.00
-Chicken Tender Basket
-$8.00
-Chili Crunch Tender Basket
-$10.00
-Crispy Chicken Sandwich
-$8.50
-Fish and Chips
-$8.50
-Garden Veggie Loaded Fries
-$8.00
-Gourmet Grilled Cheese
-$6.50
-Grilled Salmon Sandwich
-$12.00
-Korean Wings and Fries
-$12.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fresh Signature Salads
-</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Strawberry Fields Salad
-$7.25</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Suite Dinner Entree
-</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Chicken Pomodoro Pasta
-$7.00
-Chicken Potato Gnocchi
-$7.50
-Rigatoni with Beef Bolognese
-$7.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Suite Dinner Sides
-</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Flan
-$3.00
-Garlic Bread
-$2.00</t>
+BYO Poke Bowl CV
+$11.50
+Romaine Lettuce
+Spring Mix
+Unseasoned Sticky Rice</t>
         </is>
       </c>
     </row>

</xml_diff>